<commit_message>
Ready for Qld election!
</commit_message>
<xml_diff>
--- a/python/Data/poll-data-qld.xlsx
+++ b/python/Data/poll-data-qld.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\python\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42C6F372-7FA8-4046-BE89-F19670FE831C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5449EDBC-808C-4192-837D-D7AD93BEB34C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="1815" windowWidth="33540" windowHeight="19785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13290" yWindow="3795" windowWidth="24255" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="18">
   <si>
     <t>MidDate</t>
   </si>
@@ -85,6 +84,9 @@
   </si>
   <si>
     <t>F2F Morgan</t>
+  </si>
+  <si>
+    <t>Morgan SMS</t>
   </si>
 </sst>
 </file>
@@ -411,12 +413,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U197"/>
+  <dimension ref="A1:U200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="600" activePane="bottomLeft"/>
+      <pane ySplit="600" topLeftCell="A178" activePane="bottomLeft"/>
       <selection activeCell="J1" sqref="J1:J1048576"/>
-      <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
+      <selection pane="bottomLeft" activeCell="D191" sqref="D191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6784,6 +6786,102 @@
         <v>3</v>
       </c>
     </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>44116</v>
+      </c>
+      <c r="B198" t="s">
+        <v>2</v>
+      </c>
+      <c r="C198">
+        <v>52</v>
+      </c>
+      <c r="D198" s="6">
+        <v>37</v>
+      </c>
+      <c r="E198" s="6">
+        <v>37</v>
+      </c>
+      <c r="F198" s="6">
+        <v>11</v>
+      </c>
+      <c r="G198" s="6">
+        <v>9</v>
+      </c>
+      <c r="H198" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I198" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J198">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>44125</v>
+      </c>
+      <c r="B199" t="s">
+        <v>17</v>
+      </c>
+      <c r="C199">
+        <v>51</v>
+      </c>
+      <c r="D199" s="6">
+        <v>35</v>
+      </c>
+      <c r="E199" s="6">
+        <v>36</v>
+      </c>
+      <c r="F199" s="6">
+        <v>10</v>
+      </c>
+      <c r="G199" s="6">
+        <v>12</v>
+      </c>
+      <c r="H199" s="6">
+        <v>2</v>
+      </c>
+      <c r="I199" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J199" s="6">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>44132</v>
+      </c>
+      <c r="B200" t="s">
+        <v>2</v>
+      </c>
+      <c r="C200">
+        <v>51.5</v>
+      </c>
+      <c r="D200" s="6">
+        <v>36</v>
+      </c>
+      <c r="E200" s="6">
+        <v>37</v>
+      </c>
+      <c r="F200" s="6">
+        <v>11</v>
+      </c>
+      <c r="G200" s="6">
+        <v>10</v>
+      </c>
+      <c r="H200" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I200" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J200" s="6">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>